<commit_message>
add dynamic calculation of page limit
</commit_message>
<xml_diff>
--- a/final_windows_executable/input.xlsx
+++ b/final_windows_executable/input.xlsx
@@ -682,8 +682,8 @@
     <col width="10.125" customWidth="1" style="5" min="5" max="170"/>
     <col width="10.875" customWidth="1" style="5" min="171" max="521"/>
     <col width="11" customWidth="1" style="5" min="522" max="522"/>
-    <col width="10.875" customWidth="1" style="5" min="523" max="541"/>
-    <col width="10.875" customWidth="1" style="5" min="542" max="16384"/>
+    <col width="10.875" customWidth="1" style="5" min="523" max="542"/>
+    <col width="10.875" customWidth="1" style="5" min="543" max="16384"/>
   </cols>
   <sheetData>
     <row r="2" ht="45" customHeight="1">
@@ -745,68 +745,68 @@
       <c r="E7" s="3" t="n"/>
     </row>
     <row r="8" ht="44.1" customHeight="1">
-      <c r="B8" s="23" t="inlineStr">
+      <c r="B8" s="14" t="inlineStr">
         <is>
           <t>0/77</t>
         </is>
       </c>
-      <c r="C8" s="22" t="inlineStr">
+      <c r="C8" s="13" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/company/mark/</t>
         </is>
       </c>
-      <c r="D8" s="24" t="inlineStr">
+      <c r="D8" s="15" t="inlineStr">
         <is>
           <t>Mark</t>
         </is>
       </c>
     </row>
     <row r="9" ht="44.1" customHeight="1">
-      <c r="B9" s="23" t="inlineStr">
-        <is>
-          <t>1/72</t>
-        </is>
-      </c>
-      <c r="C9" s="22" t="inlineStr">
+      <c r="B9" s="14" t="inlineStr">
+        <is>
+          <t>0/72</t>
+        </is>
+      </c>
+      <c r="C9" s="13" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/company/timeneon/</t>
         </is>
       </c>
-      <c r="D9" s="24" t="inlineStr">
+      <c r="D9" s="15" t="inlineStr">
         <is>
           <t>Neon</t>
         </is>
       </c>
     </row>
     <row r="10" ht="44.1" customHeight="1">
-      <c r="B10" s="23" t="inlineStr">
-        <is>
-          <t>1/10</t>
-        </is>
-      </c>
-      <c r="C10" s="22" t="inlineStr">
+      <c r="B10" s="14" t="inlineStr">
+        <is>
+          <t>0/10</t>
+        </is>
+      </c>
+      <c r="C10" s="13" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/company/distrito.me/</t>
         </is>
       </c>
-      <c r="D10" s="24" t="inlineStr">
+      <c r="D10" s="15" t="inlineStr">
         <is>
           <t>Distrito</t>
         </is>
       </c>
     </row>
     <row r="11" ht="44.1" customHeight="1">
-      <c r="B11" s="23" t="inlineStr">
+      <c r="B11" s="14" t="inlineStr">
         <is>
           <t>1/28</t>
         </is>
       </c>
-      <c r="C11" s="22" t="inlineStr">
+      <c r="C11" s="13" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/company/liv-up/</t>
         </is>
       </c>
-      <c r="D11" s="24" t="inlineStr">
+      <c r="D11" s="15" t="inlineStr">
         <is>
           <t>Liv Up</t>
         </is>
@@ -1144,7 +1144,7 @@
   <dimension ref="B2:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B10:B11"/>
+      <selection activeCell="B11" sqref="B8:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15.75" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
fix dynamic page limit
</commit_message>
<xml_diff>
--- a/final_windows_executable/input.xlsx
+++ b/final_windows_executable/input.xlsx
@@ -745,68 +745,68 @@
       <c r="E7" s="3" t="n"/>
     </row>
     <row r="8" ht="44.1" customHeight="1">
-      <c r="B8" s="14" t="inlineStr">
-        <is>
-          <t>0/77</t>
-        </is>
-      </c>
-      <c r="C8" s="13" t="inlineStr">
+      <c r="B8" s="23" t="inlineStr">
+        <is>
+          <t>2/77</t>
+        </is>
+      </c>
+      <c r="C8" s="22" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/company/mark/</t>
         </is>
       </c>
-      <c r="D8" s="15" t="inlineStr">
+      <c r="D8" s="24" t="inlineStr">
         <is>
           <t>Mark</t>
         </is>
       </c>
     </row>
     <row r="9" ht="44.1" customHeight="1">
-      <c r="B9" s="14" t="inlineStr">
-        <is>
-          <t>0/72</t>
-        </is>
-      </c>
-      <c r="C9" s="13" t="inlineStr">
+      <c r="B9" s="23" t="inlineStr">
+        <is>
+          <t>3/72</t>
+        </is>
+      </c>
+      <c r="C9" s="22" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/company/timeneon/</t>
         </is>
       </c>
-      <c r="D9" s="15" t="inlineStr">
+      <c r="D9" s="24" t="inlineStr">
         <is>
           <t>Neon</t>
         </is>
       </c>
     </row>
     <row r="10" ht="44.1" customHeight="1">
-      <c r="B10" s="14" t="inlineStr">
-        <is>
-          <t>0/10</t>
-        </is>
-      </c>
-      <c r="C10" s="13" t="inlineStr">
+      <c r="B10" s="23" t="inlineStr">
+        <is>
+          <t>3/10</t>
+        </is>
+      </c>
+      <c r="C10" s="22" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/company/distrito.me/</t>
         </is>
       </c>
-      <c r="D10" s="15" t="inlineStr">
+      <c r="D10" s="24" t="inlineStr">
         <is>
           <t>Distrito</t>
         </is>
       </c>
     </row>
     <row r="11" ht="44.1" customHeight="1">
-      <c r="B11" s="14" t="inlineStr">
-        <is>
-          <t>1/28</t>
-        </is>
-      </c>
-      <c r="C11" s="13" t="inlineStr">
+      <c r="B11" s="23" t="inlineStr">
+        <is>
+          <t>3/28</t>
+        </is>
+      </c>
+      <c r="C11" s="22" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/company/liv-up/</t>
         </is>
       </c>
-      <c r="D11" s="15" t="inlineStr">
+      <c r="D11" s="24" t="inlineStr">
         <is>
           <t>Liv Up</t>
         </is>

</xml_diff>

<commit_message>
add 999 response check
</commit_message>
<xml_diff>
--- a/final_windows_executable/input.xlsx
+++ b/final_windows_executable/input.xlsx
@@ -682,8 +682,8 @@
     <col width="10.125" customWidth="1" style="5" min="5" max="170"/>
     <col width="10.875" customWidth="1" style="5" min="171" max="521"/>
     <col width="11" customWidth="1" style="5" min="522" max="522"/>
-    <col width="10.875" customWidth="1" style="5" min="523" max="542"/>
-    <col width="10.875" customWidth="1" style="5" min="543" max="16384"/>
+    <col width="10.875" customWidth="1" style="5" min="523" max="543"/>
+    <col width="10.875" customWidth="1" style="5" min="544" max="16384"/>
   </cols>
   <sheetData>
     <row r="2" ht="45" customHeight="1">
@@ -745,68 +745,68 @@
       <c r="E7" s="3" t="n"/>
     </row>
     <row r="8" ht="44.1" customHeight="1">
-      <c r="B8" s="23" t="inlineStr">
+      <c r="B8" s="14" t="inlineStr">
         <is>
           <t>2/77</t>
         </is>
       </c>
-      <c r="C8" s="22" t="inlineStr">
+      <c r="C8" s="13" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/company/mark/</t>
         </is>
       </c>
-      <c r="D8" s="24" t="inlineStr">
+      <c r="D8" s="15" t="inlineStr">
         <is>
           <t>Mark</t>
         </is>
       </c>
     </row>
     <row r="9" ht="44.1" customHeight="1">
-      <c r="B9" s="23" t="inlineStr">
+      <c r="B9" s="14" t="inlineStr">
         <is>
           <t>3/72</t>
         </is>
       </c>
-      <c r="C9" s="22" t="inlineStr">
+      <c r="C9" s="13" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/company/timeneon/</t>
         </is>
       </c>
-      <c r="D9" s="24" t="inlineStr">
+      <c r="D9" s="15" t="inlineStr">
         <is>
           <t>Neon</t>
         </is>
       </c>
     </row>
     <row r="10" ht="44.1" customHeight="1">
-      <c r="B10" s="23" t="inlineStr">
+      <c r="B10" s="14" t="inlineStr">
         <is>
           <t>3/10</t>
         </is>
       </c>
-      <c r="C10" s="22" t="inlineStr">
+      <c r="C10" s="13" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/company/distrito.me/</t>
         </is>
       </c>
-      <c r="D10" s="24" t="inlineStr">
+      <c r="D10" s="15" t="inlineStr">
         <is>
           <t>Distrito</t>
         </is>
       </c>
     </row>
     <row r="11" ht="44.1" customHeight="1">
-      <c r="B11" s="23" t="inlineStr">
+      <c r="B11" s="14" t="inlineStr">
         <is>
           <t>3/28</t>
         </is>
       </c>
-      <c r="C11" s="22" t="inlineStr">
+      <c r="C11" s="13" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/company/liv-up/</t>
         </is>
       </c>
-      <c r="D11" s="24" t="inlineStr">
+      <c r="D11" s="15" t="inlineStr">
         <is>
           <t>Liv Up</t>
         </is>
@@ -1144,7 +1144,7 @@
   <dimension ref="B2:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B8:B11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15.75" outlineLevelCol="0"/>

</xml_diff>